<commit_message>
Laura: Dokument Wochenziele aktualisiert. Leider hat Eclipse mir verwehrt in die altuelle GUI hineinzusehen, weshalb dort die TODOs nicht gut mit eingeabreitet werden konnten.
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -7,40 +7,17 @@
     <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
   </bookViews>
   <sheets>
-    <sheet name="Pausenplan" sheetId="1" r:id="rId1"/>
+    <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Pausenplan!$A$1:$H$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Wochenpläne!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Satisfied Microsoft Office customer</author>
-  </authors>
-  <commentList>
-    <comment ref="F3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="8"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Geben Sie das Datum für Montag dieser Woche ein. Das Enddatum wird automatisch angezeigt.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Name </t>
   </si>
@@ -96,9 +73,6 @@
     <t>Thomas</t>
   </si>
   <si>
-    <t>ab 18.12.11 Ebenen Haus 5 einlesen und überprüfen ob alles richtig eingetragen wurde</t>
-  </si>
-  <si>
     <t>bis 18.12.11 Datenbank: Testen ob Teile von Wörtern erkannt werden und dementsprechend Datenbank anlegen</t>
   </si>
   <si>
@@ -106,6 +80,124 @@
   </si>
   <si>
     <t>Plan über Wochenziele</t>
+  </si>
+  <si>
+    <t>Datenbank to-do:</t>
+  </si>
+  <si>
+    <t>integer einführen</t>
+  </si>
+  <si>
+    <t>Multitouch</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>A1: Pflichtenheft anpassen (Buttons, Textausgabe, Klickstream) 
+A2: SA fertig machen</t>
+  </si>
+  <si>
+    <t>A1: David: Testen ob Buttons auf drehbarem Canvas noch klickbar</t>
+  </si>
+  <si>
+    <t>A1: Ausfühliche Recherche wie werden einzelne Test (Klassentest, Modultests &amp; Integrationstest) konkret umgesetzt
+A2: Erstellung Testprotokoll für Pathfinding
+A3: Erstellung Testprogramm Pathfinding (eventuell automatische Tests, die direkt ins Testprotokoll schreiben)</t>
+  </si>
+  <si>
+    <t>Testprogramm für Datenbank erstellen, was überprüft ob Knoten untereinander verbunden sind (via Nachba-Ids) in beiden Richtungen (Vorschlag von David)</t>
+  </si>
+  <si>
+    <t>ab 18.12.11 Ebenen Haus 5 einlesen und überprüfen ob alles richtig eingetragen wurde - verzögert durch verzögerung in der Datenbankvorstellung</t>
+  </si>
+  <si>
+    <t>noch unbestimmt</t>
+  </si>
+  <si>
+    <t>Teamlegende:</t>
+  </si>
+  <si>
+    <t>GUI: Thomas und Eric, welche für das graphical user interface zuständig sind</t>
+  </si>
+  <si>
+    <t>GO: Eric und Nils welche für die Klasse Graphical Output zuständig sind</t>
+  </si>
+  <si>
+    <t>PM: Laura, Projektmanagement</t>
+  </si>
+  <si>
+    <t>GD: Laura, Grafikdesign</t>
+  </si>
+  <si>
+    <t>A1: Alle ebenen anlegen als Rohformat erstellen  - funktionen einführen drawFloorX() (Z.B. "Haus3 Ebene 2" anzeigen lassen anstatt grafische Darstellung der Ebenen)</t>
+  </si>
+  <si>
+    <t>A1: je nach ergebnissen von David (Ziel2, GUI, A1) Buttons designen oder eben nicht
+A2: genauerer Designentwurf als das was im Pflichtenheft vorhanden ist, Absprache mit Eric</t>
+  </si>
+  <si>
+    <t>A1: restliche Klassentests nach Vorarbeit in Ziel 2 QA vorbereiten, nicht vergessen - absprache mit jeweiligen Klassenverantwortlichen halten</t>
+  </si>
+  <si>
+    <t>A1:Grafik aus Pflichtenheft anpassen an vorgaben von PM und Pfeile einzeichnen, wie Bilder zusammenhängen</t>
+  </si>
+  <si>
+    <t>A1: fiktive Knoten aus dem Prototypen vom Format her auf Datenbank anpassen (Attribute) für Datenbanktest</t>
+  </si>
+  <si>
+    <t>Pathfinding/Nils</t>
+  </si>
+  <si>
+    <t>nicht vergessen Version von UASJ-Maps zu speichern. Bei Problemen bitte unbedingt melden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laura </t>
+  </si>
+  <si>
+    <t>Helfen bei GO: Datenbank erstellen, Aufgabenverteilung von Nils erwartet :)</t>
+  </si>
+  <si>
+    <t>A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)
+A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)
+A3: je nach Ergebnissen von David (Ziel2, GUI, A1) Buttonlistener einführen</t>
+  </si>
+  <si>
+    <t>A1: Problem Singeltouch lösen
+A2: Ebenen von Haus 5 und einem weiteren Haus grafisch darstellen
+A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) 
+A4: in der setFloor() restliche frie Navi umsetzen (Häuser auf Campus)
+A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
+  </si>
+  <si>
+    <t>Farblegende:</t>
+  </si>
+  <si>
+    <t>grün</t>
+  </si>
+  <si>
+    <t>erledigt</t>
+  </si>
+  <si>
+    <t>rot</t>
+  </si>
+  <si>
+    <t>nicht erledigt</t>
+  </si>
+  <si>
+    <t>blau</t>
+  </si>
+  <si>
+    <t>nicht erledigt Aufgrund von Abhängigkeit zu anderen Aufgaben, die nicht erfüllt wurden - wir erledigt sobald andere Aufgaben erledigt</t>
+  </si>
+  <si>
+    <t>QA: Sascha, welcher für die Quality Assurance zuständig ist</t>
   </si>
 </sst>
 </file>
@@ -113,10 +205,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="d\a\t\um\,\ \k\u\r\z"/>
-    <numFmt numFmtId="169" formatCode="\Fes\t"/>
+    <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
+    <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -227,8 +319,38 @@
     </font>
     <font>
       <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -288,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -495,38 +617,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="22"/>
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color indexed="23"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="23"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="22"/>
-      </right>
-      <top style="thin">
-        <color indexed="23"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -572,20 +672,20 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -601,7 +701,7 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -650,42 +750,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="10" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -696,18 +760,87 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:I30"/>
+  <dimension ref="B2:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -1086,13 +1219,13 @@
     <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="1.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="2" customFormat="1" ht="43.5" customHeight="1">
+    <row r="2" spans="2:15" s="2" customFormat="1" ht="43.5" customHeight="1">
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
@@ -1102,10 +1235,14 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="2:9" ht="21" customHeight="1">
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="2:15" ht="21" customHeight="1">
       <c r="B3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -1122,8 +1259,11 @@
         <v>40934</v>
       </c>
       <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="2:9" ht="17.100000000000001" customHeight="1">
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1133,25 +1273,25 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:9" ht="15.95" customHeight="1">
+    <row r="5" spans="2:15" ht="15.95" customHeight="1">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="46">
         <v>40899</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="46">
         <v>40906</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="2:15" ht="17.100000000000001" customHeight="1">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1162,112 +1302,134 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="56"/>
-      <c r="H6" s="57"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="61"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:9" ht="22.5">
-      <c r="B7" s="60" t="s">
+    <row r="7" spans="2:15" ht="22.5">
+      <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="67" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="23"/>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="61"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="63"/>
+      <c r="F7" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:9" ht="23.25" customHeight="1">
-      <c r="B8" s="60" t="s">
+    <row r="8" spans="2:15" ht="60" customHeight="1">
+      <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="63"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="2:15" ht="111" customHeight="1">
+      <c r="B9" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="63"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="2:15" ht="39" customHeight="1">
+      <c r="B10" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="63"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="2:15" ht="50.25" customHeight="1">
+      <c r="B11" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="24"/>
-    </row>
-    <row r="9" spans="2:9" ht="22.5">
-      <c r="B9" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B10" s="60" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="2:15" ht="37.5" customHeight="1">
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="63"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" spans="2:15" ht="39" customHeight="1">
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-    </row>
-    <row r="11" spans="2:9" ht="33.75">
-      <c r="B11" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="F13" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="63"/>
+      <c r="H13" s="64"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
+    <row r="14" spans="2:15" ht="17.100000000000001" customHeight="1">
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="26"/>
       <c r="E14" s="27"/>
       <c r="F14" s="24"/>
@@ -1275,18 +1437,18 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:9" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="2:15" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="46">
         <v>40913</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="46">
         <v>40920</v>
       </c>
       <c r="G15" s="42" t="s">
@@ -1294,8 +1456,11 @@
       </c>
       <c r="H15" s="43"/>
       <c r="I15" s="31"/>
-    </row>
-    <row r="16" spans="2:9" ht="17.100000000000001" customHeight="1">
+      <c r="L15" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="17.100000000000001" customHeight="1">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1306,173 +1471,281 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="55"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B17" s="60" t="s">
+    <row r="17" spans="2:12" ht="78.75">
+      <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="60" t="s">
+      <c r="C17" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="2:12" ht="146.25">
+      <c r="B18" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="49"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="2:12" ht="45">
+      <c r="B19" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="49"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="2:12" ht="56.25">
+      <c r="B20" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="2:12" ht="45">
+      <c r="B21" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="2:12" ht="22.5">
+      <c r="B22" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+    </row>
+    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
+      <c r="B24" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="46">
+        <v>40927</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="46">
+        <v>40934</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="43"/>
+      <c r="I24" s="31"/>
+      <c r="L24" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B25" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="54"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="25"/>
+    </row>
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="52"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="18" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B18" s="60" t="s">
+      <c r="C26" s="38"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="24"/>
+    </row>
+    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="60" t="s">
+      <c r="C27" s="37"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B19" s="60" t="s">
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="24"/>
+    </row>
+    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="60" t="s">
+      <c r="C28" s="37"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="2:9" s="29" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B21" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="58">
-        <v>40927</v>
-      </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="58">
-        <v>40934</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="43"/>
-      <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B22" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="25"/>
-    </row>
-    <row r="23" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B23" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="52"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="24"/>
-    </row>
-    <row r="24" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B24" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="24"/>
-    </row>
-    <row r="25" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B25" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="24"/>
-    </row>
-    <row r="26" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B26" s="24"/>
-    </row>
-    <row r="27" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B27" s="24"/>
-    </row>
-    <row r="28" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B28" s="24"/>
-    </row>
-    <row r="29" spans="2:9" ht="17.100000000000001" customHeight="1">
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="24"/>
+    </row>
+    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B29" s="24"/>
     </row>
-    <row r="30" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B30" s="24"/>
     </row>
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B31" s="24"/>
+    </row>
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="74"/>
+      <c r="I33" s="75"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" s="76"/>
+      <c r="I34" s="75"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="77"/>
+      <c r="I35" s="78"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="70" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="67.5">
+      <c r="B42" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="73" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F25:H25"/>
     <mergeCell ref="F19:H19"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1482,6 +1755,5 @@
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Laura: Plan über Wochenziele UASJ-Maps
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -7,40 +7,17 @@
     <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
   </bookViews>
   <sheets>
-    <sheet name="Pausenplan" sheetId="1" r:id="rId1"/>
+    <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Pausenplan!$A$1:$H$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Wochenpläne!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Satisfied Microsoft Office customer</author>
-  </authors>
-  <commentList>
-    <comment ref="F3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="8"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Geben Sie das Datum für Montag dieser Woche ein. Das Enddatum wird automatisch angezeigt.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>Name </t>
   </si>
@@ -96,9 +73,6 @@
     <t>Thomas</t>
   </si>
   <si>
-    <t>ab 18.12.11 Ebenen Haus 5 einlesen und überprüfen ob alles richtig eingetragen wurde</t>
-  </si>
-  <si>
     <t>bis 18.12.11 Datenbank: Testen ob Teile von Wörtern erkannt werden und dementsprechend Datenbank anlegen</t>
   </si>
   <si>
@@ -106,6 +80,124 @@
   </si>
   <si>
     <t>Plan über Wochenziele</t>
+  </si>
+  <si>
+    <t>Datenbank to-do:</t>
+  </si>
+  <si>
+    <t>integer einführen</t>
+  </si>
+  <si>
+    <t>Multitouch</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>A1: Pflichtenheft anpassen (Buttons, Textausgabe, Klickstream) 
+A2: SA fertig machen</t>
+  </si>
+  <si>
+    <t>A1: David: Testen ob Buttons auf drehbarem Canvas noch klickbar</t>
+  </si>
+  <si>
+    <t>A1: Ausfühliche Recherche wie werden einzelne Test (Klassentest, Modultests &amp; Integrationstest) konkret umgesetzt
+A2: Erstellung Testprotokoll für Pathfinding
+A3: Erstellung Testprogramm Pathfinding (eventuell automatische Tests, die direkt ins Testprotokoll schreiben)</t>
+  </si>
+  <si>
+    <t>Testprogramm für Datenbank erstellen, was überprüft ob Knoten untereinander verbunden sind (via Nachba-Ids) in beiden Richtungen (Vorschlag von David)</t>
+  </si>
+  <si>
+    <t>ab 18.12.11 Ebenen Haus 5 einlesen und überprüfen ob alles richtig eingetragen wurde - verzögert durch verzögerung in der Datenbankvorstellung</t>
+  </si>
+  <si>
+    <t>noch unbestimmt</t>
+  </si>
+  <si>
+    <t>Teamlegende:</t>
+  </si>
+  <si>
+    <t>GUI: Thomas und Eric, welche für das graphical user interface zuständig sind</t>
+  </si>
+  <si>
+    <t>GO: Eric und Nils welche für die Klasse Graphical Output zuständig sind</t>
+  </si>
+  <si>
+    <t>PM: Laura, Projektmanagement</t>
+  </si>
+  <si>
+    <t>GD: Laura, Grafikdesign</t>
+  </si>
+  <si>
+    <t>A1: Alle ebenen anlegen als Rohformat erstellen  - funktionen einführen drawFloorX() (Z.B. "Haus3 Ebene 2" anzeigen lassen anstatt grafische Darstellung der Ebenen)</t>
+  </si>
+  <si>
+    <t>A1: je nach ergebnissen von David (Ziel2, GUI, A1) Buttons designen oder eben nicht
+A2: genauerer Designentwurf als das was im Pflichtenheft vorhanden ist, Absprache mit Eric</t>
+  </si>
+  <si>
+    <t>A1: restliche Klassentests nach Vorarbeit in Ziel 2 QA vorbereiten, nicht vergessen - absprache mit jeweiligen Klassenverantwortlichen halten</t>
+  </si>
+  <si>
+    <t>A1:Grafik aus Pflichtenheft anpassen an vorgaben von PM und Pfeile einzeichnen, wie Bilder zusammenhängen</t>
+  </si>
+  <si>
+    <t>A1: fiktive Knoten aus dem Prototypen vom Format her auf Datenbank anpassen (Attribute) für Datenbanktest</t>
+  </si>
+  <si>
+    <t>Pathfinding/Nils</t>
+  </si>
+  <si>
+    <t>nicht vergessen Version von UASJ-Maps zu speichern. Bei Problemen bitte unbedingt melden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laura </t>
+  </si>
+  <si>
+    <t>Helfen bei GO: Datenbank erstellen, Aufgabenverteilung von Nils erwartet :)</t>
+  </si>
+  <si>
+    <t>A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)
+A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)
+A3: je nach Ergebnissen von David (Ziel2, GUI, A1) Buttonlistener einführen</t>
+  </si>
+  <si>
+    <t>A1: Problem Singeltouch lösen
+A2: Ebenen von Haus 5 und einem weiteren Haus grafisch darstellen
+A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) 
+A4: in der setFloor() restliche frie Navi umsetzen (Häuser auf Campus)
+A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
+  </si>
+  <si>
+    <t>Farblegende:</t>
+  </si>
+  <si>
+    <t>grün</t>
+  </si>
+  <si>
+    <t>erledigt</t>
+  </si>
+  <si>
+    <t>rot</t>
+  </si>
+  <si>
+    <t>nicht erledigt</t>
+  </si>
+  <si>
+    <t>blau</t>
+  </si>
+  <si>
+    <t>nicht erledigt Aufgrund von Abhängigkeit zu anderen Aufgaben, die nicht erfüllt wurden - wir erledigt sobald andere Aufgaben erledigt</t>
+  </si>
+  <si>
+    <t>QA: Sascha, welcher für die Quality Assurance zuständig ist</t>
   </si>
 </sst>
 </file>
@@ -113,10 +205,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="d\a\t\um\,\ \k\u\r\z"/>
-    <numFmt numFmtId="169" formatCode="\Fes\t"/>
+    <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
+    <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -227,8 +319,38 @@
     </font>
     <font>
       <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -288,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -495,38 +617,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="22"/>
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color indexed="23"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="23"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="22"/>
-      </right>
-      <top style="thin">
-        <color indexed="23"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -572,20 +672,20 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -601,7 +701,7 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -650,42 +750,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="10" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -696,18 +760,87 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:I30"/>
+  <dimension ref="B2:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -1086,13 +1219,13 @@
     <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="1.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="2" customFormat="1" ht="43.5" customHeight="1">
+    <row r="2" spans="2:15" s="2" customFormat="1" ht="43.5" customHeight="1">
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
@@ -1102,10 +1235,14 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="2:9" ht="21" customHeight="1">
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="2:15" ht="21" customHeight="1">
       <c r="B3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -1122,8 +1259,11 @@
         <v>40934</v>
       </c>
       <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="2:9" ht="17.100000000000001" customHeight="1">
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1133,25 +1273,25 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:9" ht="15.95" customHeight="1">
+    <row r="5" spans="2:15" ht="15.95" customHeight="1">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="46">
         <v>40899</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="58">
+      <c r="F5" s="46">
         <v>40906</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="2:15" ht="17.100000000000001" customHeight="1">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1162,112 +1302,134 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="56"/>
-      <c r="H6" s="57"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="61"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:9" ht="22.5">
-      <c r="B7" s="60" t="s">
+    <row r="7" spans="2:15" ht="22.5">
+      <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="67" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="23"/>
-      <c r="E7" s="60" t="s">
+      <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="61"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="63"/>
+      <c r="F7" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:9" ht="23.25" customHeight="1">
-      <c r="B8" s="60" t="s">
+    <row r="8" spans="2:15" ht="60" customHeight="1">
+      <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="63"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="2:15" ht="111" customHeight="1">
+      <c r="B9" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="63"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="2:15" ht="39" customHeight="1">
+      <c r="B10" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="63"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="2:15" ht="50.25" customHeight="1">
+      <c r="B11" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="24"/>
-    </row>
-    <row r="9" spans="2:9" ht="22.5">
-      <c r="B9" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="46"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B10" s="60" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="63"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="2:15" ht="37.5" customHeight="1">
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="63"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" spans="2:15" ht="39" customHeight="1">
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-    </row>
-    <row r="11" spans="2:9" ht="33.75">
-      <c r="B11" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="F13" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="63"/>
+      <c r="H13" s="64"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
+    <row r="14" spans="2:15" ht="17.100000000000001" customHeight="1">
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="26"/>
       <c r="E14" s="27"/>
       <c r="F14" s="24"/>
@@ -1275,18 +1437,18 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:9" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="2:15" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="46">
         <v>40913</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="46">
         <v>40920</v>
       </c>
       <c r="G15" s="42" t="s">
@@ -1294,8 +1456,11 @@
       </c>
       <c r="H15" s="43"/>
       <c r="I15" s="31"/>
-    </row>
-    <row r="16" spans="2:9" ht="17.100000000000001" customHeight="1">
+      <c r="L15" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="17.100000000000001" customHeight="1">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1306,173 +1471,281 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="55"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B17" s="60" t="s">
+    <row r="17" spans="2:12" ht="78.75">
+      <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="60" t="s">
+      <c r="C17" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="2:12" ht="146.25">
+      <c r="B18" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="49"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="2:12" ht="45">
+      <c r="B19" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="49"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="2:12" ht="56.25">
+      <c r="B20" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="2:12" ht="45">
+      <c r="B21" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="2:12" ht="22.5">
+      <c r="B22" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+    </row>
+    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
+      <c r="B24" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="46">
+        <v>40927</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="46">
+        <v>40934</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="43"/>
+      <c r="I24" s="31"/>
+      <c r="L24" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B25" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="32"/>
+      <c r="E25" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="54"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="25"/>
+    </row>
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="52"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="18" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B18" s="60" t="s">
+      <c r="C26" s="38"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="24"/>
+    </row>
+    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="60" t="s">
+      <c r="C27" s="37"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B19" s="60" t="s">
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="24"/>
+    </row>
+    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="60" t="s">
+      <c r="C28" s="37"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="2:9" s="29" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B21" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="58">
-        <v>40927</v>
-      </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="58">
-        <v>40934</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="43"/>
-      <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B22" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="50"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="25"/>
-    </row>
-    <row r="23" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B23" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="52"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="24"/>
-    </row>
-    <row r="24" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B24" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="60" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="24"/>
-    </row>
-    <row r="25" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B25" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="24"/>
-    </row>
-    <row r="26" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B26" s="24"/>
-    </row>
-    <row r="27" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B27" s="24"/>
-    </row>
-    <row r="28" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B28" s="24"/>
-    </row>
-    <row r="29" spans="2:9" ht="17.100000000000001" customHeight="1">
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="24"/>
+    </row>
+    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B29" s="24"/>
     </row>
-    <row r="30" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B30" s="24"/>
     </row>
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B31" s="24"/>
+    </row>
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="74"/>
+      <c r="I33" s="75"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" s="76"/>
+      <c r="I34" s="75"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="77"/>
+      <c r="I35" s="78"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="70" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="67.5">
+      <c r="B42" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="73" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F25:H25"/>
     <mergeCell ref="F19:H19"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1482,6 +1755,5 @@
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Laura: Update Plan über Wochenziele UASJ-Maps.xlsx
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Name </t>
   </si>
@@ -80,12 +80,6 @@
   </si>
   <si>
     <t>Plan über Wochenziele</t>
-  </si>
-  <si>
-    <t>Datenbank to-do:</t>
-  </si>
-  <si>
-    <t>integer einführen</t>
   </si>
   <si>
     <t>Multitouch</t>
@@ -112,19 +106,10 @@
 A3: Erstellung Testprogramm Pathfinding (eventuell automatische Tests, die direkt ins Testprotokoll schreiben)</t>
   </si>
   <si>
-    <t>Testprogramm für Datenbank erstellen, was überprüft ob Knoten untereinander verbunden sind (via Nachba-Ids) in beiden Richtungen (Vorschlag von David)</t>
-  </si>
-  <si>
     <t>ab 18.12.11 Ebenen Haus 5 einlesen und überprüfen ob alles richtig eingetragen wurde - verzögert durch verzögerung in der Datenbankvorstellung</t>
   </si>
   <si>
-    <t>noch unbestimmt</t>
-  </si>
-  <si>
     <t>Teamlegende:</t>
-  </si>
-  <si>
-    <t>GUI: Thomas und Eric, welche für das graphical user interface zuständig sind</t>
   </si>
   <si>
     <t>GO: Eric und Nils welche für die Klasse Graphical Output zuständig sind</t>
@@ -194,10 +179,19 @@
     <t>blau</t>
   </si>
   <si>
-    <t>nicht erledigt Aufgrund von Abhängigkeit zu anderen Aufgaben, die nicht erfüllt wurden - wir erledigt sobald andere Aufgaben erledigt</t>
-  </si>
-  <si>
     <t>QA: Sascha, welcher für die Quality Assurance zuständig ist</t>
+  </si>
+  <si>
+    <t>nicht erledigt Aufgrund von Abhängigkeit zu anderen Aufgaben, die nicht erfüllt wurden - wird erledigt sobald andere Aufgaben erledigt</t>
+  </si>
+  <si>
+    <t>Testprogramm für Datenbank erstellen, was überprüft ob Knoten untereinander verbunden sind (via Nachbar-Ids) in beiden Richtungen (Vorschlag von David)</t>
+  </si>
+  <si>
+    <t>GUI: Thomas und David, welche für das Graphical User Interface zuständig sind</t>
+  </si>
+  <si>
+    <t>noch unbestimmt (wird zeitnah geklärt, wer das machen soll)</t>
   </si>
 </sst>
 </file>
@@ -634,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -764,51 +758,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -841,6 +790,54 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1204,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O42"/>
+  <dimension ref="B2:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -1223,7 +1220,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="2" customFormat="1" ht="43.5" customHeight="1">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1235,12 +1232,9 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="3"/>
-      <c r="N2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="2:15" ht="21" customHeight="1">
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="2:14" ht="21" customHeight="1">
       <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
@@ -1259,11 +1253,8 @@
         <v>40934</v>
       </c>
       <c r="I3" s="15"/>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="17.100000000000001" customHeight="1">
+    </row>
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1273,7 +1264,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:15" ht="15.95" customHeight="1">
+    <row r="5" spans="2:14" ht="15.95" customHeight="1">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
@@ -1291,7 +1282,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:15" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1302,132 +1293,132 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="60"/>
-      <c r="H6" s="61"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="78"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:15" ht="22.5">
+    <row r="7" spans="2:14" ht="22.5">
       <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="52" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="63"/>
-      <c r="H7" s="64"/>
+      <c r="F7" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="74"/>
+      <c r="H7" s="75"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:15" ht="60" customHeight="1">
+    <row r="8" spans="2:14" ht="60" customHeight="1">
       <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="68" t="s">
-        <v>31</v>
+      <c r="C8" s="53" t="s">
+        <v>28</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="63"/>
-      <c r="H8" s="64"/>
+      <c r="F8" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="74"/>
+      <c r="H8" s="75"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:15" ht="111" customHeight="1">
+    <row r="9" spans="2:14" ht="111" customHeight="1">
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="51" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="64"/>
+      <c r="F9" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="74"/>
+      <c r="H9" s="75"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="2:15" ht="39" customHeight="1">
+    <row r="10" spans="2:14" ht="39" customHeight="1">
       <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="51" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="62" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="64"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:15" ht="50.25" customHeight="1">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1">
       <c r="B11" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="52" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="63"/>
-      <c r="H11" s="64"/>
+        <v>24</v>
+      </c>
+      <c r="F11" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="74"/>
+      <c r="H11" s="75"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:15" ht="37.5" customHeight="1">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1">
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="62" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="64"/>
+        <v>38</v>
+      </c>
+      <c r="F12" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="74"/>
+      <c r="H12" s="75"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:15" ht="39" customHeight="1">
+    <row r="13" spans="2:14" ht="39" customHeight="1">
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="26"/>
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="63"/>
-      <c r="H13" s="64"/>
+      <c r="F13" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="74"/>
+      <c r="H13" s="75"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:15" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="26"/>
@@ -1437,7 +1428,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:15" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
@@ -1457,10 +1448,10 @@
       <c r="H15" s="43"/>
       <c r="I15" s="31"/>
       <c r="L15" s="29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="17.100000000000001" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1471,11 +1462,11 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="54"/>
-      <c r="H16" s="55"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="69"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="78.75">
@@ -1483,13 +1474,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="58"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="72"/>
       <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:12" ht="146.25">
@@ -1497,13 +1488,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="52"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="66"/>
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:12" ht="45">
@@ -1511,55 +1502,55 @@
         <v>8</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="66"/>
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="2:12" ht="56.25">
       <c r="B20" s="48" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="49"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
       <c r="I20" s="24"/>
     </row>
     <row r="21" spans="2:12" ht="45">
-      <c r="B21" s="48" t="s">
-        <v>32</v>
+      <c r="B21" s="79" t="s">
+        <v>54</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="49"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
       <c r="I21" s="24"/>
     </row>
     <row r="22" spans="2:12" ht="22.5">
       <c r="B22" s="48" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="49"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
       <c r="I22" s="24"/>
     </row>
     <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1592,7 +1583,7 @@
       <c r="H24" s="43"/>
       <c r="I24" s="31"/>
       <c r="L24" s="29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1606,11 +1597,11 @@
       <c r="E25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="53" t="s">
+      <c r="F25" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="54"/>
-      <c r="H25" s="55"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="69"/>
       <c r="I25" s="25"/>
     </row>
     <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1622,9 +1613,9 @@
       <c r="E26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="56"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="58"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="72"/>
       <c r="I26" s="24"/>
     </row>
     <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1636,9 +1627,9 @@
       <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="52"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="66"/>
       <c r="I27" s="24"/>
     </row>
     <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1650,9 +1641,9 @@
       <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="52"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="66"/>
       <c r="I28" s="24"/>
     </row>
     <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1666,67 +1657,67 @@
     </row>
     <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
       <c r="B33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H33" s="74"/>
-      <c r="I33" s="75"/>
+        <v>53</v>
+      </c>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
     </row>
     <row r="34" spans="2:9">
       <c r="B34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H34" s="76"/>
-      <c r="I34" s="75"/>
+        <v>30</v>
+      </c>
+      <c r="H34" s="61"/>
+      <c r="I34" s="60"/>
     </row>
     <row r="35" spans="2:9">
       <c r="B35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H35" s="77"/>
-      <c r="I35" s="78"/>
+        <v>50</v>
+      </c>
+      <c r="H35" s="62"/>
+      <c r="I35" s="63"/>
     </row>
     <row r="36" spans="2:9">
       <c r="B36" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:9">
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="2:9">
       <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="67.5">
+      <c r="B42" s="57" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="B40" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="70" t="s">
+      <c r="C42" s="58" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9">
-      <c r="B41" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="70" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="67.5">
-      <c r="B42" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="73" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nils: GraphicalOutput: - Funktionsgerüste für alle möglichen Ebenen erstellt - Default-Canvas jeder Ebene erstellt, sodass ersichtlich ist, welche Ebene theoretisch gerade angezeigt wird (Falls mal irgendwann eine nicht vorhandenen ID ausgewählt wird, dann wird das auf dem Canvas als Meldung ausgegeben) - set_floor erweitert, dass Auswahl der Häsuer auf Campusanzeige möglich ist (Code beachten, siehe Kommentare). Derzeit Sprung auf Ebene 0 jedes Hauses
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
+    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -154,55 +154,75 @@
 A3: je nach Ergebnissen von David (Ziel2, GUI, A1) Buttonlistener einführen</t>
   </si>
   <si>
-    <t>A1: Problem Singeltouch lösen
+    <t>Farblegende:</t>
+  </si>
+  <si>
+    <t>grün</t>
+  </si>
+  <si>
+    <t>erledigt</t>
+  </si>
+  <si>
+    <t>rot</t>
+  </si>
+  <si>
+    <t>nicht erledigt</t>
+  </si>
+  <si>
+    <t>blau</t>
+  </si>
+  <si>
+    <t>QA: Sascha, welcher für die Quality Assurance zuständig ist</t>
+  </si>
+  <si>
+    <t>nicht erledigt Aufgrund von Abhängigkeit zu anderen Aufgaben, die nicht erfüllt wurden - wird erledigt sobald andere Aufgaben erledigt</t>
+  </si>
+  <si>
+    <t>Testprogramm für Datenbank erstellen, was überprüft ob Knoten untereinander verbunden sind (via Nachbar-Ids) in beiden Richtungen (Vorschlag von David)</t>
+  </si>
+  <si>
+    <t>GUI: Thomas und David, welche für das Graphical User Interface zuständig sind</t>
+  </si>
+  <si>
+    <t>noch unbestimmt (wird zeitnah geklärt, wer das machen soll)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: Problem Singeltouch lösen
 A2: Ebenen von Haus 5 und einem weiteren Haus grafisch darstellen
 A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) 
-A4: in der setFloor() restliche frie Navi umsetzen (Häuser auf Campus)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A4: in der setFloor() restliche frie Navi umsetzen (Häuser auf Campus)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
-  </si>
-  <si>
-    <t>Farblegende:</t>
-  </si>
-  <si>
-    <t>grün</t>
-  </si>
-  <si>
-    <t>erledigt</t>
-  </si>
-  <si>
-    <t>rot</t>
-  </si>
-  <si>
-    <t>nicht erledigt</t>
-  </si>
-  <si>
-    <t>blau</t>
-  </si>
-  <si>
-    <t>QA: Sascha, welcher für die Quality Assurance zuständig ist</t>
-  </si>
-  <si>
-    <t>nicht erledigt Aufgrund von Abhängigkeit zu anderen Aufgaben, die nicht erfüllt wurden - wird erledigt sobald andere Aufgaben erledigt</t>
-  </si>
-  <si>
-    <t>Testprogramm für Datenbank erstellen, was überprüft ob Knoten untereinander verbunden sind (via Nachbar-Ids) in beiden Richtungen (Vorschlag von David)</t>
-  </si>
-  <si>
-    <t>GUI: Thomas und David, welche für das Graphical User Interface zuständig sind</t>
-  </si>
-  <si>
-    <t>noch unbestimmt (wird zeitnah geklärt, wer das machen soll)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -345,6 +365,12 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -628,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -791,6 +817,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -818,26 +865,8 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,11 +942,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -991,6 +1025,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1025,6 +1060,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1200,27 +1236,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1234,7 +1270,7 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1">
+    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
@@ -1254,7 +1290,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1264,7 +1300,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.95" customHeight="1">
+    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
@@ -1282,7 +1318,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1293,14 +1329,14 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="76" t="s">
+      <c r="F6" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="77"/>
-      <c r="H6" s="78"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="70"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="22.5">
+    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
@@ -1311,14 +1347,14 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="75"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="67"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1">
+    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
@@ -1329,14 +1365,14 @@
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="73" t="s">
+      <c r="F8" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="74"/>
-      <c r="H8" s="75"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="67"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1">
+    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
@@ -1347,14 +1383,14 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="F9" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="74"/>
-      <c r="H9" s="75"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1">
+    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
@@ -1365,14 +1401,14 @@
       <c r="E10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="73" t="s">
+      <c r="F10" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="74"/>
-      <c r="H10" s="75"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="67"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="48" t="s">
         <v>17</v>
       </c>
@@ -1383,42 +1419,42 @@
       <c r="E11" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="F11" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="74"/>
-      <c r="H11" s="75"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="73" t="s">
+      <c r="F12" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="74"/>
-      <c r="H12" s="75"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="67"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1">
+    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="26"/>
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="74"/>
-      <c r="H13" s="75"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="67"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="26"/>
@@ -1428,7 +1464,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
@@ -1451,7 +1487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1462,14 +1498,14 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="68"/>
-      <c r="H16" s="69"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="76"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="78.75">
+    <row r="17" spans="2:12" ht="71.400000000000006" x14ac:dyDescent="0.25">
       <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
@@ -1478,26 +1514,26 @@
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="72"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="79"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="146.25">
+    <row r="18" spans="2:12" ht="132.6" x14ac:dyDescent="0.25">
       <c r="B18" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="66"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="73"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="45">
+    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
       <c r="B19" s="48" t="s">
         <v>8</v>
       </c>
@@ -1506,12 +1542,12 @@
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="66"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="73"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="56.25">
+    <row r="20" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="B20" s="48" t="s">
         <v>24</v>
       </c>
@@ -1525,12 +1561,12 @@
       <c r="H20" s="50"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="45">
-      <c r="B21" s="79" t="s">
-        <v>54</v>
+    <row r="21" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
+      <c r="B21" s="64" t="s">
+        <v>53</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="49"/>
@@ -1539,7 +1575,7 @@
       <c r="H21" s="50"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="22.5">
+    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B22" s="48" t="s">
         <v>40</v>
       </c>
@@ -1553,7 +1589,7 @@
       <c r="H22" s="50"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="26"/>
@@ -1563,7 +1599,7 @@
       <c r="H23" s="33"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="39" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="44" t="s">
         <v>5</v>
       </c>
@@ -1597,14 +1633,14 @@
       <c r="E25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="67" t="s">
+      <c r="F25" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="68"/>
-      <c r="H25" s="69"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="76"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="48" t="s">
         <v>6</v>
       </c>
@@ -1613,12 +1649,12 @@
       <c r="E26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="70"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="72"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="79"/>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="48" t="s">
         <v>7</v>
       </c>
@@ -1627,12 +1663,12 @@
       <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="64"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="66"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="73"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="48" t="s">
         <v>8</v>
       </c>
@@ -1641,87 +1677,95 @@
       <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="64"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="66"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="73"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="24"/>
     </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H33" s="59"/>
       <c r="I33" s="60"/>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H34" s="61"/>
       <c r="I34" s="60"/>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H35" s="62"/>
       <c r="I35" s="63"/>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="54" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="B40" s="54" t="s">
+      <c r="C40" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="55" t="s">
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="56" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="2:9">
-      <c r="B41" s="56" t="s">
+      <c r="C41" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="55" t="s">
+    </row>
+    <row r="42" spans="2:9" ht="66" x14ac:dyDescent="0.25">
+      <c r="B42" s="57" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" ht="67.5">
-      <c r="B42" s="57" t="s">
-        <v>49</v>
-      </c>
       <c r="C42" s="58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F19:H19"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
@@ -1730,14 +1774,6 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F19:H19"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
David: Wochenziele: done: Ziel2: GUI: A1 edited: Ziel3: GUI: A3 added: Ziel3: GUI: A4
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
+    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>David</author>
+  </authors>
+  <commentList>
+    <comment ref="F7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Nein, das ist nicht möglich.
+Weiteres Vorgehen siehe Ziel3 -&gt; GUI -&gt; A3</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
@@ -147,11 +182,6 @@
   </si>
   <si>
     <t>Helfen bei GO: Datenbank erstellen, Aufgabenverteilung von Nils erwartet :)</t>
-  </si>
-  <si>
-    <t>A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)
-A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)
-A3: je nach Ergebnissen von David (Ziel2, GUI, A1) Buttonlistener einführen</t>
   </si>
   <si>
     <t>Farblegende:</t>
@@ -213,16 +243,22 @@
 A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
     </r>
   </si>
+  <si>
+    <t>A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)
+A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)
+A3: David: Singletouch für Campusdarstellung erstellen: Wo wurde gedrückt?
+A4: Menüführung fertig machen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -371,6 +407,19 @@
       <sz val="9"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -654,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -821,6 +870,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -838,34 +914,13 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -951,7 +1006,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1025,7 +1080,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1060,7 +1114,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1236,27 +1289,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1270,7 +1323,7 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="21" customHeight="1">
       <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
@@ -1290,7 +1343,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1300,7 +1353,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="15.95" customHeight="1">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
@@ -1318,7 +1371,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1329,14 +1382,14 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="70"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="79"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="22.5">
       <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
@@ -1347,14 +1400,14 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="67"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="82"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="60" customHeight="1">
       <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
@@ -1368,11 +1421,11 @@
       <c r="F8" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="66"/>
-      <c r="H8" s="67"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="76"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="111" customHeight="1">
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
@@ -1383,14 +1436,14 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="66"/>
-      <c r="H9" s="67"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="76"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="39" customHeight="1">
       <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
@@ -1401,14 +1454,14 @@
       <c r="E10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="66"/>
-      <c r="H10" s="67"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1">
       <c r="B11" s="48" t="s">
         <v>17</v>
       </c>
@@ -1419,42 +1472,42 @@
       <c r="E11" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="66"/>
-      <c r="H11" s="67"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1">
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="F12" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="76"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" ht="39" customHeight="1">
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="26"/>
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="76"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="26"/>
@@ -1464,7 +1517,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
@@ -1487,7 +1540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1498,42 +1551,42 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="74" t="s">
+      <c r="F16" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="75"/>
-      <c r="H16" s="76"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="71.400000000000006" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="101.25">
       <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="79"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="132.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="146.25">
       <c r="B18" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="73"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="67"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="45">
       <c r="B19" s="48" t="s">
         <v>8</v>
       </c>
@@ -1542,12 +1595,12 @@
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="73"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="67"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="56.25">
       <c r="B20" s="48" t="s">
         <v>24</v>
       </c>
@@ -1561,12 +1614,12 @@
       <c r="H20" s="50"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="45">
       <c r="B21" s="64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="49"/>
@@ -1575,7 +1628,7 @@
       <c r="H21" s="50"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="22.5">
       <c r="B22" s="48" t="s">
         <v>40</v>
       </c>
@@ -1589,7 +1642,7 @@
       <c r="H22" s="50"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="26"/>
@@ -1599,7 +1652,7 @@
       <c r="H23" s="33"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B24" s="39" t="s">
         <v>3</v>
       </c>
@@ -1622,7 +1675,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B25" s="44" t="s">
         <v>5</v>
       </c>
@@ -1633,14 +1686,14 @@
       <c r="E25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="74" t="s">
+      <c r="F25" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="75"/>
-      <c r="H25" s="76"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="70"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B26" s="48" t="s">
         <v>6</v>
       </c>
@@ -1649,12 +1702,12 @@
       <c r="E26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="73"/>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B27" s="48" t="s">
         <v>7</v>
       </c>
@@ -1663,12 +1716,12 @@
       <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="71"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="73"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="67"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B28" s="48" t="s">
         <v>8</v>
       </c>
@@ -1677,87 +1730,95 @@
       <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="71"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="73"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="67"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B30" s="24"/>
     </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H33" s="59"/>
       <c r="I33" s="60"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H34" s="61"/>
       <c r="I34" s="60"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H35" s="62"/>
       <c r="I35" s="63"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9">
       <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="54" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="54" t="s">
+      <c r="C40" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="55" t="s">
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="56" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="56" t="s">
+      <c r="C41" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="55" t="s">
+    </row>
+    <row r="42" spans="2:9" ht="67.5">
+      <c r="B42" s="57" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" ht="66" x14ac:dyDescent="0.25">
-      <c r="B42" s="57" t="s">
-        <v>48</v>
-      </c>
       <c r="C42" s="58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F16:H16"/>
@@ -1766,14 +1827,6 @@
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
@@ -1782,5 +1835,6 @@
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Laura: Wochenziele PM und GD sowie A1 von QA, Verknüpfung UML und SA verbal beschrieben, Ordner QA angelegt
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -136,11 +136,6 @@
     <t>A1: David: Testen ob Buttons auf drehbarem Canvas noch klickbar</t>
   </si>
   <si>
-    <t>A1: Ausfühliche Recherche wie werden einzelne Test (Klassentest, Modultests &amp; Integrationstest) konkret umgesetzt
-A2: Erstellung Testprotokoll für Pathfinding
-A3: Erstellung Testprogramm Pathfinding (eventuell automatische Tests, die direkt ins Testprotokoll schreiben)</t>
-  </si>
-  <si>
     <t>ab 18.12.11 Ebenen Haus 5 einlesen und überprüfen ob alles richtig eingetragen wurde - verzögert durch verzögerung in der Datenbankvorstellung</t>
   </si>
   <si>
@@ -248,6 +243,28 @@
 A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)
 A3: David: Singletouch für Campusdarstellung erstellen: Wo wurde gedrückt?
 A4: Menüführung fertig machen</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: Ausfühliche Recherche wie werden einzelne Test (Klassentest, Modultests &amp; Integrationstest) konkret umgesetzt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A2: Erstellung Testprotokoll für Pathfinding
+A3: Erstellung Testprogramm Pathfinding (eventuell automatische Tests, die direkt ins Testprotokoll schreiben)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -870,6 +887,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -895,33 +939,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,7 +1310,7 @@
   <dimension ref="B2:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:H7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -1382,11 +1399,11 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="77" t="s">
+      <c r="F6" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="78"/>
-      <c r="H6" s="79"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="70"/>
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:14" ht="22.5">
@@ -1400,11 +1417,11 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="80" t="s">
+      <c r="F7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="81"/>
-      <c r="H7" s="82"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="73"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="2:14" ht="60" customHeight="1">
@@ -1412,17 +1429,17 @@
         <v>7</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="75"/>
-      <c r="H8" s="76"/>
+      <c r="F8" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="66"/>
+      <c r="H8" s="67"/>
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="2:14" ht="111" customHeight="1">
@@ -1436,29 +1453,29 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="75"/>
-      <c r="H9" s="76"/>
+      <c r="F9" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="66"/>
+      <c r="H9" s="67"/>
       <c r="I9" s="24"/>
     </row>
     <row r="10" spans="2:14" ht="39" customHeight="1">
       <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="52" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="74" t="s">
+      <c r="F10" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="75"/>
-      <c r="H10" s="76"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="73"/>
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="2:14" ht="50.25" customHeight="1">
@@ -1472,11 +1489,11 @@
       <c r="E11" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="76"/>
+      <c r="F11" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="72"/>
+      <c r="H11" s="73"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="2:14" ht="37.5" customHeight="1">
@@ -1484,13 +1501,13 @@
       <c r="C12" s="49"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="75"/>
-      <c r="H12" s="76"/>
+      <c r="F12" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="66"/>
+      <c r="H12" s="67"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="2:14" ht="39" customHeight="1">
@@ -1500,11 +1517,11 @@
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="74" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="75"/>
-      <c r="H13" s="76"/>
+      <c r="F13" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="66"/>
+      <c r="H13" s="67"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
@@ -1551,11 +1568,11 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="68" t="s">
+      <c r="F16" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="69"/>
-      <c r="H16" s="70"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="79"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="101.25">
@@ -1563,13 +1580,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="82"/>
       <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:12" ht="146.25">
@@ -1577,13 +1594,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="67"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="76"/>
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:12" ht="45">
@@ -1591,13 +1608,13 @@
         <v>8</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="67"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="76"/>
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="2:12" ht="56.25">
@@ -1605,7 +1622,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="49"/>
@@ -1616,10 +1633,10 @@
     </row>
     <row r="21" spans="2:12" ht="45">
       <c r="B21" s="64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="49"/>
@@ -1630,10 +1647,10 @@
     </row>
     <row r="22" spans="2:12" ht="22.5">
       <c r="B22" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="47" t="s">
         <v>40</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>41</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="49"/>
@@ -1686,11 +1703,11 @@
       <c r="E25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="68" t="s">
+      <c r="F25" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="69"/>
-      <c r="H25" s="70"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="79"/>
       <c r="I25" s="25"/>
     </row>
     <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1702,9 +1719,9 @@
       <c r="E26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="71"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="73"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="82"/>
       <c r="I26" s="24"/>
     </row>
     <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1716,9 +1733,9 @@
       <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="65"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="67"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="76"/>
       <c r="I27" s="24"/>
     </row>
     <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1730,9 +1747,9 @@
       <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="65"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="67"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="76"/>
       <c r="I28" s="24"/>
     </row>
     <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1746,71 +1763,79 @@
     </row>
     <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
       <c r="B33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H33" s="59"/>
       <c r="I33" s="60"/>
     </row>
     <row r="34" spans="2:9">
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H34" s="61"/>
       <c r="I34" s="60"/>
     </row>
     <row r="35" spans="2:9">
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H35" s="62"/>
       <c r="I35" s="63"/>
     </row>
     <row r="36" spans="2:9">
       <c r="B36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:9">
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="2:9">
       <c r="B39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="2:9">
       <c r="B40" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="55" t="s">
         <v>43</v>
-      </c>
-      <c r="C40" s="55" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:9">
       <c r="B41" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="55" t="s">
         <v>45</v>
-      </c>
-      <c r="C41" s="55" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="67.5">
       <c r="B42" s="57" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F19:H19"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
@@ -1819,14 +1844,6 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F19:H19"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Nils: Modul Database: - ist nun fertig. Als Datenbank dient die Testumgebung des Prototypen. Knoten von 0-7 - Eingabe über Eingabefelder möglich - Ausgabe über Konsole - Knoten an Datenbankarbeit angepasst - Pathfinding an Datenbankarbeit angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
+    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -270,12 +270,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -887,6 +887,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -903,42 +939,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,7 +1023,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1097,6 +1097,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1131,6 +1132,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1306,27 +1308,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1340,7 +1342,7 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1">
+    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
@@ -1360,7 +1362,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1370,7 +1372,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.95" customHeight="1">
+    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
@@ -1388,7 +1390,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1399,14 +1401,14 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="70"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="82"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="22.5">
+    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
@@ -1417,14 +1419,14 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="71" t="s">
+      <c r="F7" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="72"/>
-      <c r="H7" s="73"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="76"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1">
+    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
@@ -1435,14 +1437,14 @@
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="66"/>
-      <c r="H8" s="67"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="79"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1">
+    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
@@ -1453,14 +1455,14 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="66"/>
-      <c r="H9" s="67"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="79"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1">
+    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
@@ -1471,14 +1473,14 @@
       <c r="E10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="71" t="s">
+      <c r="F10" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="73"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="48" t="s">
         <v>17</v>
       </c>
@@ -1489,42 +1491,42 @@
       <c r="E11" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="72"/>
-      <c r="H11" s="73"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="F12" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="76"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1">
+    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="26"/>
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="26"/>
@@ -1534,7 +1536,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +1559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1568,14 +1570,14 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="77" t="s">
+      <c r="F16" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="78"/>
-      <c r="H16" s="79"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="101.25">
+    <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
       <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
@@ -1584,12 +1586,12 @@
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="82"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="146.25">
+    <row r="18" spans="2:12" ht="132.6" x14ac:dyDescent="0.25">
       <c r="B18" s="48" t="s">
         <v>7</v>
       </c>
@@ -1598,12 +1600,12 @@
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="76"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="67"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="45">
+    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
       <c r="B19" s="48" t="s">
         <v>8</v>
       </c>
@@ -1612,12 +1614,12 @@
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="76"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="67"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="56.25">
+    <row r="20" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="B20" s="48" t="s">
         <v>24</v>
       </c>
@@ -1631,7 +1633,7 @@
       <c r="H20" s="50"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="45">
+    <row r="21" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="B21" s="64" t="s">
         <v>51</v>
       </c>
@@ -1645,7 +1647,7 @@
       <c r="H21" s="50"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="22.5">
+    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B22" s="48" t="s">
         <v>39</v>
       </c>
@@ -1659,7 +1661,7 @@
       <c r="H22" s="50"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="26"/>
@@ -1669,7 +1671,7 @@
       <c r="H23" s="33"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="39" t="s">
         <v>3</v>
       </c>
@@ -1692,7 +1694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="44" t="s">
         <v>5</v>
       </c>
@@ -1703,14 +1705,14 @@
       <c r="E25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="77" t="s">
+      <c r="F25" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="78"/>
-      <c r="H25" s="79"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="70"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="48" t="s">
         <v>6</v>
       </c>
@@ -1719,12 +1721,12 @@
       <c r="E26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="80"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="82"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="73"/>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="48" t="s">
         <v>7</v>
       </c>
@@ -1733,12 +1735,12 @@
       <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="74"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="76"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="67"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="48" t="s">
         <v>8</v>
       </c>
@@ -1747,62 +1749,62 @@
       <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="76"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="67"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="24"/>
     </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H33" s="59"/>
       <c r="I33" s="60"/>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H34" s="61"/>
       <c r="I34" s="60"/>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H35" s="62"/>
       <c r="I35" s="63"/>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="54" t="s">
         <v>42</v>
       </c>
@@ -1810,7 +1812,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="56" t="s">
         <v>44</v>
       </c>
@@ -1818,7 +1820,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="67.5">
+    <row r="42" spans="2:9" ht="66" x14ac:dyDescent="0.25">
       <c r="B42" s="57" t="s">
         <v>46</v>
       </c>
@@ -1828,6 +1830,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F16:H16"/>
@@ -1836,14 +1846,6 @@
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
David: GUI: hab an onResume gearbeitet, aber nicht exceptions nicht lösen können
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
+    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -47,6 +47,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="C17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A3: Funktionen in GO noch nicht vorhanden</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -239,12 +263,6 @@
     </r>
   </si>
   <si>
-    <t>A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)
-A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)
-A3: David: Singletouch für Campusdarstellung erstellen: Wo wurde gedrückt?
-A4: Menüführung fertig machen</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="9"/>
@@ -266,16 +284,42 @@
 A3: Erstellung Testprogramm Pathfinding (eventuell automatische Tests, die direkt ins Testprotokoll schreiben)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)
+A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: David: Singletouch für Campusdarstellung erstellen: Wo wurde gedrückt?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A4: Menüführung fertig machen</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -886,6 +930,33 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -912,33 +983,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,7 +1067,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1097,7 +1141,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1132,7 +1175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1308,27 +1350,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:H11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1342,7 +1384,7 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="21" customHeight="1">
       <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
@@ -1362,7 +1404,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1372,7 +1414,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="15.95" customHeight="1">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1432,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1401,14 +1443,14 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="81"/>
-      <c r="H6" s="82"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="73"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="22.5">
       <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
@@ -1419,14 +1461,14 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="74" t="s">
+      <c r="F7" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="75"/>
-      <c r="H7" s="76"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="67"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="60" customHeight="1">
       <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
@@ -1437,14 +1479,14 @@
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="74" t="s">
+      <c r="F8" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="78"/>
-      <c r="H8" s="79"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="70"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="111" customHeight="1">
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
@@ -1455,14 +1497,14 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="78"/>
-      <c r="H9" s="79"/>
+      <c r="F9" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="69"/>
+      <c r="H9" s="70"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="39" customHeight="1">
       <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
@@ -1473,14 +1515,14 @@
       <c r="E10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="74" t="s">
+      <c r="F10" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="75"/>
-      <c r="H10" s="76"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="67"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1">
       <c r="B11" s="48" t="s">
         <v>17</v>
       </c>
@@ -1491,42 +1533,42 @@
       <c r="E11" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="74" t="s">
+      <c r="F11" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="76"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1">
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="74" t="s">
+      <c r="F12" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="75"/>
-      <c r="H12" s="76"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="67"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" ht="39" customHeight="1">
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="26"/>
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="70"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="26"/>
@@ -1536,7 +1578,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
@@ -1559,7 +1601,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1570,28 +1612,28 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="68" t="s">
+      <c r="F16" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="69"/>
-      <c r="H16" s="70"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="79"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="101.25">
       <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="82"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="132.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="146.25">
       <c r="B18" s="48" t="s">
         <v>7</v>
       </c>
@@ -1600,12 +1642,12 @@
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="67"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="76"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="45">
       <c r="B19" s="48" t="s">
         <v>8</v>
       </c>
@@ -1614,12 +1656,12 @@
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="67"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="76"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="56.25">
       <c r="B20" s="48" t="s">
         <v>24</v>
       </c>
@@ -1633,7 +1675,7 @@
       <c r="H20" s="50"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="45">
       <c r="B21" s="64" t="s">
         <v>51</v>
       </c>
@@ -1647,7 +1689,7 @@
       <c r="H21" s="50"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="22.5">
       <c r="B22" s="48" t="s">
         <v>39</v>
       </c>
@@ -1661,7 +1703,7 @@
       <c r="H22" s="50"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
       <c r="D23" s="26"/>
@@ -1671,7 +1713,7 @@
       <c r="H23" s="33"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B24" s="39" t="s">
         <v>3</v>
       </c>
@@ -1694,7 +1736,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B25" s="44" t="s">
         <v>5</v>
       </c>
@@ -1705,14 +1747,14 @@
       <c r="E25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="68" t="s">
+      <c r="F25" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="69"/>
-      <c r="H25" s="70"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="79"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B26" s="48" t="s">
         <v>6</v>
       </c>
@@ -1721,12 +1763,12 @@
       <c r="E26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="71"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="73"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="82"/>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B27" s="48" t="s">
         <v>7</v>
       </c>
@@ -1735,12 +1777,12 @@
       <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="65"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="67"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="76"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B28" s="48" t="s">
         <v>8</v>
       </c>
@@ -1749,62 +1791,62 @@
       <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="65"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="67"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="76"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B30" s="24"/>
     </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H33" s="59"/>
       <c r="I33" s="60"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9">
       <c r="B34" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H34" s="61"/>
       <c r="I34" s="60"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H35" s="62"/>
       <c r="I35" s="63"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9">
       <c r="B37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" s="54" t="s">
         <v>42</v>
       </c>
@@ -1812,7 +1854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" s="56" t="s">
         <v>44</v>
       </c>
@@ -1820,7 +1862,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="66" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" ht="67.5">
       <c r="B42" s="57" t="s">
         <v>46</v>
       </c>
@@ -1830,6 +1872,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F19:H19"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
@@ -1838,14 +1888,6 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F19:H19"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
David: GUI: Anpassung PH und viele Kommentare
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan �ber Wochenziele UASJ-Maps.xlsx
@@ -287,7 +287,25 @@
   <si>
     <r>
       <t xml:space="preserve">A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)
-A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -307,7 +325,16 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-A4: Menüführung fertig machen</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A4: Menüführung fertig machen</t>
     </r>
   </si>
 </sst>
@@ -930,6 +957,33 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -956,33 +1010,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1354,7 +1381,7 @@
   <dimension ref="B2:N42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F17" sqref="F17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -1443,11 +1470,11 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="71" t="s">
+      <c r="F6" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="72"/>
-      <c r="H6" s="73"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="82"/>
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:14" ht="22.5">
@@ -1461,11 +1488,11 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="67"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="76"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="2:14" ht="60" customHeight="1">
@@ -1479,11 +1506,11 @@
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="65" t="s">
+      <c r="F8" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="69"/>
-      <c r="H8" s="70"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="79"/>
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="2:14" ht="111" customHeight="1">
@@ -1497,11 +1524,11 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="69"/>
-      <c r="H9" s="70"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="79"/>
       <c r="I9" s="24"/>
     </row>
     <row r="10" spans="2:14" ht="39" customHeight="1">
@@ -1515,11 +1542,11 @@
       <c r="E10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="66"/>
-      <c r="H10" s="67"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="2:14" ht="50.25" customHeight="1">
@@ -1533,11 +1560,11 @@
       <c r="E11" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="66"/>
-      <c r="H11" s="67"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="2:14" ht="37.5" customHeight="1">
@@ -1547,11 +1574,11 @@
       <c r="E12" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="65" t="s">
+      <c r="F12" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="76"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="2:14" ht="39" customHeight="1">
@@ -1561,11 +1588,11 @@
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="F13" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="69"/>
-      <c r="H13" s="70"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
@@ -1612,11 +1639,11 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="77" t="s">
+      <c r="F16" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="78"/>
-      <c r="H16" s="79"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="101.25">
@@ -1628,9 +1655,9 @@
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="48"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="82"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:12" ht="146.25">
@@ -1642,9 +1669,9 @@
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="76"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="67"/>
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:12" ht="45">
@@ -1656,9 +1683,9 @@
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="48"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="76"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="67"/>
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="2:12" ht="56.25">
@@ -1747,11 +1774,11 @@
       <c r="E25" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="77" t="s">
+      <c r="F25" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="78"/>
-      <c r="H25" s="79"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="70"/>
       <c r="I25" s="25"/>
     </row>
     <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1763,9 +1790,9 @@
       <c r="E26" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="80"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="82"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="73"/>
       <c r="I26" s="24"/>
     </row>
     <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1777,9 +1804,9 @@
       <c r="E27" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="74"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="76"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="67"/>
       <c r="I27" s="24"/>
     </row>
     <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1791,9 +1818,9 @@
       <c r="E28" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="76"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="67"/>
       <c r="I28" s="24"/>
     </row>
     <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -1872,6 +1899,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F16:H16"/>
@@ -1880,14 +1915,6 @@
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>